<commit_message>
Se añade la funcion de añadir personajes al campo de batalla,y se hace una miniminidemo
</commit_message>
<xml_diff>
--- a/Campo de batalla.xlsx
+++ b/Campo de batalla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python\PhytonMaster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\Con lo colegas\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38663A24-3D8A-4FB5-BB46-96113FB11638}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C6B942-3B0F-4754-A803-D832DEBB68D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Monstruo</t>
   </si>
@@ -141,10 +141,7 @@
     <t xml:space="preserve">Puntos de vida </t>
   </si>
   <si>
-    <t>Rampo Doyle</t>
-  </si>
-  <si>
-    <t>Cocodrilo1</t>
+    <t>Puntos de vida maximo</t>
   </si>
 </sst>
 </file>
@@ -476,391 +473,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" style="2"/>
-    <col min="12" max="12" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="2" width="13.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="2"/>
+    <col min="13" max="13" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2">
-        <v>-1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>4</v>
-      </c>
-      <c r="M2" s="2">
-        <v>-1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>3</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2">
-        <v>7</v>
-      </c>
-      <c r="S2" s="2">
-        <v>10</v>
-      </c>
-      <c r="T2" s="2">
-        <v>16</v>
-      </c>
-      <c r="U2" s="2">
-        <v>10</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0</v>
-      </c>
-      <c r="X2" s="2">
-        <v>6</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>-1</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>6</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>3</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>4</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
     </row>
-    <row r="3" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="1">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>-3</v>
-      </c>
-      <c r="N3" s="1">
-        <v>2</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>-3</v>
-      </c>
-      <c r="T3" s="1">
-        <v>10</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="X3" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>-3</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>-3</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>-3</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>-3</v>
-      </c>
-      <c r="AI3" s="1">
-        <v>-4</v>
-      </c>
-      <c r="AJ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="1">
-        <v>2</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="C10" s="3"/>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Terminada la función atacar a falta de posibles mejoras
</commit_message>
<xml_diff>
--- a/Campo de batalla.xlsx
+++ b/Campo de batalla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\Con lo colegas\PhytonMaster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C6B942-3B0F-4754-A803-D832DEBB68D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF0DE9-54A0-4889-A61C-03125F1B8473}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
-  <si>
-    <t>Monstruo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Walking/swimming/flying</t>
   </si>
@@ -138,17 +135,26 @@
     <t>Survival (WIS)</t>
   </si>
   <si>
-    <t xml:space="preserve">Puntos de vida </t>
-  </si>
-  <si>
-    <t>Puntos de vida maximo</t>
+    <t>Rampo Doyle</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Cocodrilo 1</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Healthmax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,9 +163,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,16 +203,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,209 +500,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="13.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="1"/>
+    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="9.1796875" style="1"/>
+    <col min="40" max="40" width="11.54296875" style="1" customWidth="1"/>
+    <col min="41" max="41" width="8.81640625" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>3</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>7</v>
+      </c>
+      <c r="U2" s="1">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1">
+        <v>16</v>
+      </c>
+      <c r="W2" s="1">
+        <v>10</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B3" s="3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="K3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>-3</v>
+      </c>
+      <c r="N3" s="3">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>-3</v>
+      </c>
+      <c r="T3" s="3">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="X3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>-3</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>-3</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>-4</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="3"/>
     </row>
-    <row r="3" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="D10" s="3"/>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se añade los encuentros
</commit_message>
<xml_diff>
--- a/Campo de batalla.xlsx
+++ b/Campo de batalla.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python\PhytonMaster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Espacios de trabajo\Phyton\Con lo colegas\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF0DE9-54A0-4889-A61C-03125F1B8473}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC90307-9E4C-4949-A8F8-8062CB30711B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Walking/swimming/flying</t>
   </si>
@@ -135,13 +135,7 @@
     <t>Survival (WIS)</t>
   </si>
   <si>
-    <t>Rampo Doyle</t>
-  </si>
-  <si>
     <t>Nombre</t>
-  </si>
-  <si>
-    <t>Cocodrilo 1</t>
   </si>
   <si>
     <t>Health</t>
@@ -177,10 +171,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,7 +214,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,62 +499,62 @@
   <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="9.1796875" style="1"/>
-    <col min="40" max="40" width="11.54296875" style="1" customWidth="1"/>
-    <col min="41" max="41" width="8.81640625" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.1796875" style="1"/>
+    <col min="31" max="31" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="9.140625" style="1"/>
+    <col min="40" max="40" width="11.5703125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="8.85546875" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -663,234 +659,48 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1">
-        <v>33</v>
-      </c>
-      <c r="C2" s="1">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1">
-        <v>30</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="P2" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>3</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1">
-        <v>7</v>
-      </c>
-      <c r="U2" s="1">
-        <v>10</v>
-      </c>
-      <c r="V2" s="1">
-        <v>16</v>
-      </c>
-      <c r="W2" s="1">
-        <v>10</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>6</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>7</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>4</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>6</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>4</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3">
-        <v>33</v>
-      </c>
-      <c r="E3" s="3">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>-3</v>
-      </c>
-      <c r="N3" s="3">
-        <v>2</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="R3" s="3">
-        <v>0</v>
-      </c>
-      <c r="S3" s="3">
-        <v>-3</v>
-      </c>
-      <c r="T3" s="3">
-        <v>10</v>
-      </c>
-      <c r="U3" s="3">
-        <v>0</v>
-      </c>
-      <c r="V3" s="3">
-        <v>0</v>
-      </c>
-      <c r="W3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="X3" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>-3</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>-3</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>-3</v>
-      </c>
-      <c r="AH3" s="3">
-        <v>-3</v>
-      </c>
-      <c r="AI3" s="3">
-        <v>-4</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>2</v>
-      </c>
+    <row r="2" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:38" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
     </row>
   </sheetData>

</xml_diff>